<commit_message>
Added the cost on the title. Still missing brute force run times.
</commit_message>
<xml_diff>
--- a/Trading Post Run Times.xlsx
+++ b/Trading Post Run Times.xlsx
@@ -29,19 +29,19 @@
     <t>Sample Size</t>
   </si>
   <si>
-    <t>Brute Force</t>
-  </si>
-  <si>
     <t>Trial</t>
-  </si>
-  <si>
-    <t>Divide and Conquer</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
     <t>Run Time (ms)</t>
+  </si>
+  <si>
+    <t>Brute Force - Cost: O(n^2)</t>
+  </si>
+  <si>
+    <t>Divide and Conquer - Cost: O(n^2)</t>
   </si>
 </sst>
 </file>
@@ -99,16 +99,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -422,10 +422,10 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
@@ -439,63 +439,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="I1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="E1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="I1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9">
         <v>1</v>
       </c>
       <c r="F3" s="3">
@@ -504,7 +504,7 @@
       <c r="G3" s="6">
         <v>22</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="9">
         <v>1</v>
       </c>
       <c r="J3" s="3">
@@ -515,21 +515,21 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="3">
         <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="9"/>
       <c r="F4" s="3">
         <v>200</v>
       </c>
       <c r="G4" s="6">
         <v>7</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="3">
         <v>200</v>
       </c>
@@ -538,21 +538,21 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>400</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="9"/>
       <c r="F5" s="3">
         <v>400</v>
       </c>
       <c r="G5" s="6">
         <v>85</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="3">
         <v>400</v>
       </c>
@@ -561,21 +561,21 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>600</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E6" s="9"/>
       <c r="F6" s="3">
         <v>600</v>
       </c>
       <c r="G6" s="6">
         <v>60</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="3">
         <v>600</v>
       </c>
@@ -584,21 +584,21 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>800</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="9"/>
       <c r="F7" s="3">
         <v>800</v>
       </c>
       <c r="G7" s="6">
         <v>58</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="3">
         <v>800</v>
       </c>
@@ -610,16 +610,16 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>2</v>
       </c>
       <c r="B9" s="3">
         <v>100</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7">
         <v>2</v>
       </c>
       <c r="F9" s="3">
@@ -628,7 +628,7 @@
       <c r="G9" s="6">
         <v>9</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>2</v>
       </c>
       <c r="J9" s="3">
@@ -639,21 +639,21 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="3">
         <v>200</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="3">
         <v>200</v>
       </c>
       <c r="G10" s="6">
         <v>15</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="3">
         <v>200</v>
       </c>
@@ -662,21 +662,21 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>400</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="7"/>
       <c r="F11" s="3">
         <v>400</v>
       </c>
       <c r="G11" s="6">
         <v>23</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="3">
         <v>400</v>
       </c>
@@ -685,21 +685,21 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>600</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="3">
         <v>600</v>
       </c>
       <c r="G12" s="6">
         <v>16</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="3">
         <v>600</v>
       </c>
@@ -708,21 +708,21 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="3">
         <v>800</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="7"/>
       <c r="F13" s="3">
         <v>800</v>
       </c>
       <c r="G13" s="6">
         <v>16</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="7"/>
       <c r="J13" s="3">
         <v>800</v>
       </c>
@@ -734,16 +734,16 @@
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>3</v>
       </c>
       <c r="B15" s="3">
         <v>100</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7">
         <v>3</v>
       </c>
       <c r="F15" s="3">
@@ -752,7 +752,7 @@
       <c r="G15" s="6">
         <v>15</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>3</v>
       </c>
       <c r="J15" s="3">
@@ -763,21 +763,21 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="3">
         <v>200</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="7"/>
       <c r="F16" s="3">
         <v>200</v>
       </c>
       <c r="G16" s="6">
         <v>16</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="7"/>
       <c r="J16" s="3">
         <v>200</v>
       </c>
@@ -786,21 +786,21 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="3">
         <v>400</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="7"/>
       <c r="F17" s="3">
         <v>400</v>
       </c>
       <c r="G17" s="6">
         <v>16</v>
       </c>
-      <c r="I17" s="8"/>
+      <c r="I17" s="7"/>
       <c r="J17" s="3">
         <v>400</v>
       </c>
@@ -809,21 +809,21 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="3">
         <v>600</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="3">
         <v>600</v>
       </c>
       <c r="G18" s="6">
         <v>21</v>
       </c>
-      <c r="I18" s="8"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="3">
         <v>600</v>
       </c>
@@ -832,21 +832,21 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="3">
         <v>800</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E19" s="7"/>
       <c r="F19" s="3">
         <v>800</v>
       </c>
       <c r="G19" s="6">
         <v>10</v>
       </c>
-      <c r="I19" s="8"/>
+      <c r="I19" s="7"/>
       <c r="J19" s="3">
         <v>800</v>
       </c>
@@ -858,16 +858,16 @@
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>4</v>
       </c>
       <c r="B21" s="3">
         <v>100</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="8">
+        <v>2</v>
+      </c>
+      <c r="E21" s="7">
         <v>4</v>
       </c>
       <c r="F21" s="3">
@@ -876,7 +876,7 @@
       <c r="G21" s="6">
         <v>31</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>4</v>
       </c>
       <c r="J21" s="3">
@@ -887,21 +887,21 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="3">
         <v>200</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="7"/>
       <c r="F22" s="3">
         <v>200</v>
       </c>
       <c r="G22" s="6">
         <v>20</v>
       </c>
-      <c r="I22" s="8"/>
+      <c r="I22" s="7"/>
       <c r="J22" s="3">
         <v>200</v>
       </c>
@@ -910,21 +910,21 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="3">
         <v>400</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="7"/>
       <c r="F23" s="3">
         <v>400</v>
       </c>
       <c r="G23" s="6">
         <v>23</v>
       </c>
-      <c r="I23" s="8"/>
+      <c r="I23" s="7"/>
       <c r="J23" s="3">
         <v>400</v>
       </c>
@@ -933,21 +933,21 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="3">
         <v>600</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="7"/>
       <c r="F24" s="3">
         <v>600</v>
       </c>
       <c r="G24" s="6">
         <v>31</v>
       </c>
-      <c r="I24" s="8"/>
+      <c r="I24" s="7"/>
       <c r="J24" s="3">
         <v>600</v>
       </c>
@@ -956,21 +956,21 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="3">
         <v>800</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E25" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="7"/>
       <c r="F25" s="3">
         <v>800</v>
       </c>
       <c r="G25" s="6">
         <v>0</v>
       </c>
-      <c r="I25" s="8"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="3">
         <v>800</v>
       </c>
@@ -982,16 +982,16 @@
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="8">
+      <c r="A27" s="7">
         <v>5</v>
       </c>
       <c r="B27" s="3">
         <v>100</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="8">
+        <v>2</v>
+      </c>
+      <c r="E27" s="7">
         <v>5</v>
       </c>
       <c r="F27" s="3">
@@ -1000,7 +1000,7 @@
       <c r="G27" s="6">
         <v>28</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="7">
         <v>5</v>
       </c>
       <c r="J27" s="3">
@@ -1011,21 +1011,21 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3">
         <v>200</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="7"/>
       <c r="F28" s="3">
         <v>200</v>
       </c>
       <c r="G28" s="6">
         <v>56</v>
       </c>
-      <c r="I28" s="8"/>
+      <c r="I28" s="7"/>
       <c r="J28" s="3">
         <v>200</v>
       </c>
@@ -1034,21 +1034,21 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3">
         <v>400</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E29" s="7"/>
       <c r="F29" s="3">
         <v>400</v>
       </c>
       <c r="G29" s="6">
         <v>38</v>
       </c>
-      <c r="I29" s="8"/>
+      <c r="I29" s="7"/>
       <c r="J29" s="3">
         <v>400</v>
       </c>
@@ -1057,21 +1057,21 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="3">
         <v>600</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E30" s="7"/>
       <c r="F30" s="3">
         <v>600</v>
       </c>
       <c r="G30" s="6">
         <v>40</v>
       </c>
-      <c r="I30" s="8"/>
+      <c r="I30" s="7"/>
       <c r="J30" s="3">
         <v>600</v>
       </c>
@@ -1080,21 +1080,21 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="3">
         <v>800</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="E31" s="7"/>
       <c r="F31" s="3">
         <v>800</v>
       </c>
       <c r="G31" s="6">
         <v>11</v>
       </c>
-      <c r="I31" s="8"/>
+      <c r="I31" s="7"/>
       <c r="J31" s="3">
         <v>800</v>
       </c>
@@ -1104,14 +1104,7 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I27:I31"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="E15:E19"/>
@@ -1121,7 +1114,14 @@
     <mergeCell ref="I9:I13"/>
     <mergeCell ref="I15:I19"/>
     <mergeCell ref="I21:I25"/>
-    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>